<commit_message>
added link to excel workbook
</commit_message>
<xml_diff>
--- a/combineClean.xlsx
+++ b/combineClean.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R\landfireFSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3286D23-A6F8-485B-B15B-492FD4D9AFFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB6F13AC-C476-44BF-96DF-FACDBB158C01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="885" windowWidth="24240" windowHeight="13140" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId6"/>
+    <pivotCache cacheId="0" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -15044,7 +15044,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E79E2230-3BCC-4834-A835-D0880F2CA1E1}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="2">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E79E2230-3BCC-4834-A835-D0880F2CA1E1}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="2">
   <location ref="A3:B14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField compact="0" outline="0" showAll="0">
@@ -15298,7 +15298,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5BF7FA45-DBCC-483B-8B11-4D6B241BC22E}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5BF7FA45-DBCC-483B-8B11-4D6B241BC22E}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:D80" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField showAll="0"/>
@@ -15703,7 +15703,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="1">
   <location ref="A3:C182" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
   <pivotFields count="9">
     <pivotField compact="0" outline="0" showAll="0">
@@ -16482,7 +16482,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5B0AFF42-629B-49C3-B037-FF0B515DFF73}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5B0AFF42-629B-49C3-B037-FF0B515DFF73}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A3:B14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField showAll="0"/>
@@ -16901,8 +16901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I1254"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -49534,7 +49534,7 @@
   <dimension ref="A3:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H7:N8"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -49650,7 +49650,7 @@
   <dimension ref="A3:D80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:D78"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -52708,7 +52708,7 @@
   <dimension ref="A3:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="D10" sqref="D10:F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added pivot table exercises to the conversion tab
</commit_message>
<xml_diff>
--- a/combineClean.xlsx
+++ b/combineClean.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R\landfireFSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA35CCA1-F864-4316-80AC-A5F26A80A3B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F96E1520-FB8C-48F0-B309-B812545D155D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="885" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="combineClean" sheetId="1" r:id="rId1"/>
@@ -15929,7 +15929,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I1254"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -49072,7 +49072,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FD98CB2-CB5E-41FB-B21F-E0D8E1E854F6}">
   <dimension ref="A3:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
pushing stuff from long ago...hope it's OK :)
</commit_message>
<xml_diff>
--- a/combineClean.xlsx
+++ b/combineClean.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R\landfireFSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{147645E2-B513-4CBD-A906-C48E36B04A18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4B32E29-A585-4608-A1AA-49250B12D2C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="885" windowWidth="24240" windowHeight="13140" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="885" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="combineClean" sheetId="1" r:id="rId1"/>
@@ -15929,8 +15929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I1254"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -48671,7 +48671,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C053C8C7-6436-481A-B955-2A875A7553D6}">
   <dimension ref="A3:C80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>

</xml_diff>